<commit_message>
se arregla la data para emitir polizas movilidad en QA
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision Motor Accesorio Movilidad.xlsx
+++ b/Sura/DataSource - Emision Motor Accesorio Movilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFC234F-8C53-47B9-9CD1-02F052A46048}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA997F8E-E0F9-4E25-B9D1-12865F1B98B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="182">
   <si>
     <t>Usuario</t>
   </si>
@@ -571,6 +571,15 @@
   </si>
   <si>
     <t>ZAZ123PQM031</t>
+  </si>
+  <si>
+    <t>TipoTarjeta</t>
+  </si>
+  <si>
+    <t>NumTarjetaCred</t>
+  </si>
+  <si>
+    <t>FechaVencimiento</t>
   </si>
 </sst>
 </file>
@@ -950,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:A32"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,6 +1031,15 @@
       </c>
       <c r="N1" t="s">
         <v>22</v>
+      </c>
+      <c r="O1" t="s">
+        <v>179</v>
+      </c>
+      <c r="P1" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>181</v>
       </c>
       <c r="R1" t="s">
         <v>31</v>

</xml_diff>